<commit_message>
Updating yaml for murine-sourve v0
</commit_message>
<xml_diff>
--- a/docs/murine-source/murine-source.xlsx
+++ b/docs/murine-source/murine-source.xlsx
@@ -8,11 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="room_health_status list" sheetId="2" r:id="rId2"/>
-    <sheet name="rack_setup list" sheetId="3" r:id="rId3"/>
-    <sheet name="light_cycle list" sheetId="4" r:id="rId4"/>
-    <sheet name="bedding list" sheetId="5" r:id="rId5"/>
-    <sheet name="cage_enhancements list" sheetId="6" r:id="rId6"/>
+    <sheet name="sex list" sheetId="2" r:id="rId2"/>
+    <sheet name="euthanization_method list" sheetId="3" r:id="rId3"/>
+    <sheet name="room_health_status list" sheetId="4" r:id="rId4"/>
+    <sheet name="rack_setup list" sheetId="5" r:id="rId5"/>
+    <sheet name="light_cycle list" sheetId="6" r:id="rId6"/>
+    <sheet name="bedding list" sheetId="7" r:id="rId7"/>
+    <sheet name="cage_enhancements list" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -33,11 +35,115 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Jackson Labs nomenclature. When mutant alleles are part of the strain name, use "&lt;" and "&gt;" to indicate the superscripted alleles. For example, C57BL/6J-KitW-39J should be entered as "C57BL/6J-Kit&lt;W-39J&gt;", where "W-39J" would be the portion of the string displayed as superscripted text. For further information, see the "Quick Guide to Mouse Nomenclature" (https://resources.jax.org/guides/quick-guide-to-mouse-nomenclature).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The Research Resource Identifier (RRID) (https://scicrunch.org/resources/data/source/nlx_154697-1/search) for the strain. An example is 'RRID:MGI:3713213'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The sex of the mouse.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is the source an embryo? Use either 'True' or 'False'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The date when the mouse/embryo was born/fertilized. If the hours/minutes are not known, use '00:00'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Is the source deceased? Use either 'True' or 'False'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The date when the mouse/embryo died. If the hours/minutes are not known, use '00:00'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the source was euthanized, select the method of euthanization.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>A free text description of how long mice live within the local environment. It is recommended to provide the median or maximum values for murine lifespans.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +252,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>strain_rrid</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>is_embryo</t>
+  </si>
+  <si>
+    <t>date_of_birth_or_fertilization</t>
+  </si>
+  <si>
+    <t>is_deceased</t>
+  </si>
+  <si>
+    <t>date_of_death</t>
+  </si>
+  <si>
+    <t>euthanization_method</t>
+  </si>
+  <si>
+    <t>Carbon dioxide asphixiation</t>
+  </si>
+  <si>
+    <t>Inhaled anesthetic agents</t>
+  </si>
+  <si>
+    <t>Injected anesthetic agents</t>
+  </si>
+  <si>
+    <t>Cervical dislocation</t>
+  </si>
+  <si>
+    <t>Decapitation</t>
+  </si>
+  <si>
+    <t>Hypothermia</t>
+  </si>
+  <si>
+    <t>Rapid freezing</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
   <si>
     <t>local_lifespan_data</t>
   </si>
@@ -158,9 +318,6 @@
   </si>
   <si>
     <t>Pathogen and opportunist free</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>room_temperature</t>
@@ -593,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -602,7 +759,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,46 +767,82 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." sqref="B2:B1048576">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: M / F." sqref="C2:C1048576">
+      <formula1>'sex list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="D2:D1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="F2:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from euthanization_method list." sqref="H2:H1048576">
+      <formula1>'euthanization_method list'!$A$1:$A$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." sqref="J2:J1048576">
       <formula1>'room_health_status list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="K2:K1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." sqref="L2:L1048576">
       <formula1>'rack_setup list'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." sqref="M2:M1048576">
       <formula1>'light_cycle list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." sqref="N2:N1048576">
       <formula1>'bedding list'!$A$1:$A$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." sqref="Q2:Q1048576">
       <formula1>'cage_enhancements list'!$A$1:$A$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -660,7 +853,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -668,16 +861,11 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -688,7 +876,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -696,22 +884,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -729,17 +937,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -748,6 +956,67 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -757,52 +1026,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -810,7 +1079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -820,32 +1089,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding 'source_id' to murine source spec to support bulk metadata ingestion and validation
</commit_message>
<xml_diff>
--- a/docs/murine-source/murine-source.xlsx
+++ b/docs/murine-source/murine-source.xlsx
@@ -35,11 +35,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>SenNet ID of the source (whole organism) of the assayed tissue.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Jackson Labs nomenclature. When mutant alleles are part of the strain name, use "&lt;" and "&gt;" to indicate the superscripted alleles. For example, C57BL/6J-KitW-39J should be entered as "C57BL/6J-Kit&lt;W-39J&gt;", where "W-39J" would be the portion of the string displayed as superscripted text. For further information, see the "Quick Guide to Mouse Nomenclature" (https://resources.jax.org/guides/quick-guide-to-mouse-nomenclature).</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -143,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -252,7 +265,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+  <si>
+    <t>source_id</t>
+  </si>
   <si>
     <t>strain</t>
   </si>
@@ -750,7 +766,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -759,7 +775,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -785,25 +801,25 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>43</v>
@@ -811,38 +827,41 @@
       <c r="Q1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: M / F." sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: M / F." sqref="D2:D1048576">
       <formula1>'sex list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="E2:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="G2:G1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from euthanization_method list." sqref="H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from euthanization_method list." sqref="I2:I1048576">
       <formula1>'euthanization_method list'!$A$1:$A$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Pathogen free / Pathogen and opportunist free / Other." sqref="K2:K1048576">
       <formula1>'room_health_status list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="K2:K1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="L2:L1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Biocontainment / Ventilated / Micro-Isolator / Conventional." sqref="M2:M1048576">
       <formula1>'rack_setup list'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." sqref="M2:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Standard/default / Longer photoperiods / Reverse light cycles." sqref="N2:N1048576">
       <formula1>'light_cycle list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." sqref="N2:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from bedding list." sqref="O2:O1048576">
       <formula1>'bedding list'!$A$1:$A$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." sqref="Q2:Q1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from cage_enhancements list." sqref="R2:R1048576">
       <formula1>'cage_enhancements list'!$A$1:$A$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -861,12 +880,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -884,42 +903,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -937,17 +956,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -965,22 +984,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -998,17 +1017,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1026,52 +1045,52 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1089,32 +1108,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>